<commit_message>
3d -> 2d started
</commit_message>
<xml_diff>
--- a/output/concentrations/ds.5p.ser/big_ser_test_res.xlsx
+++ b/output/concentrations/ds.5p.ser/big_ser_test_res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
   <si>
     <t>H</t>
   </si>
@@ -37,7 +37,37 @@
     <t>DNA</t>
   </si>
   <si>
-    <t>log10.K.</t>
+    <t>prod_names</t>
+  </si>
+  <si>
+    <t>H+PO4</t>
+  </si>
+  <si>
+    <t>2H+PO4</t>
+  </si>
+  <si>
+    <t>3H+PO4</t>
+  </si>
+  <si>
+    <t>H+PO4+Cu</t>
+  </si>
+  <si>
+    <t>2H+2PO4+Cu</t>
+  </si>
+  <si>
+    <t>2H+PO4+Cu</t>
+  </si>
+  <si>
+    <t>4H+2PO4+Cu</t>
+  </si>
+  <si>
+    <t>2Hydr+Cu</t>
+  </si>
+  <si>
+    <t>Cu+DNA</t>
+  </si>
+  <si>
+    <t>lg_k</t>
   </si>
   <si>
     <t>tot</t>
@@ -56,33 +86,6 @@
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>H+PO4</t>
-  </si>
-  <si>
-    <t>2H+PO4</t>
-  </si>
-  <si>
-    <t>3H+PO4</t>
-  </si>
-  <si>
-    <t>H+PO4+Cu</t>
-  </si>
-  <si>
-    <t>2H+2PO4+Cu</t>
-  </si>
-  <si>
-    <t>2H+PO4+Cu</t>
-  </si>
-  <si>
-    <t>4H+2PO4+Cu</t>
-  </si>
-  <si>
-    <t>2Hydr+Cu</t>
-  </si>
-  <si>
-    <t>Cu+DNA</t>
   </si>
   <si>
     <t>p(Hydr)</t>
@@ -479,13 +482,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +504,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,8 +524,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -535,8 +544,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -552,8 +564,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -569,8 +584,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2</v>
       </c>
@@ -586,8 +604,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2</v>
       </c>
@@ -603,8 +624,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>4</v>
       </c>
@@ -620,8 +644,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>-1</v>
       </c>
@@ -637,8 +664,11 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>0</v>
       </c>
@@ -654,8 +684,11 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>0</v>
       </c>
@@ -671,8 +704,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>0</v>
       </c>
@@ -687,6 +723,9 @@
       </c>
       <c r="E12">
         <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +743,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -777,19 +816,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -809,7 +848,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -829,7 +868,7 @@
         <v>1e-19</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -849,7 +888,7 @@
         <v>1e-19</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -869,7 +908,7 @@
         <v>1e-19</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -889,7 +928,7 @@
         <v>1e-19</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -909,7 +948,7 @@
         <v>1e-19</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -929,7 +968,7 @@
         <v>1e-19</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -949,7 +988,7 @@
         <v>1e-19</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -969,7 +1008,7 @@
         <v>1e-19</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -989,7 +1028,7 @@
         <v>1e-19</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1009,7 +1048,7 @@
         <v>8.500000000000001e-05</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1029,7 +1068,7 @@
         <v>8.500000000000001e-05</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1062,25 +1101,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
@@ -1089,13 +1128,13 @@
         <v>2</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1103,19 +1142,19 @@
         <v>5.471930600758359e-08</v>
       </c>
       <c r="B2">
-        <v>4.356481401231425e-06</v>
+        <v>4.356481401231417e-06</v>
       </c>
       <c r="C2">
         <v>8.259517860200998e-05</v>
       </c>
       <c r="D2">
-        <v>1.081213216203394e-09</v>
+        <v>1.081213216202099e-09</v>
       </c>
       <c r="E2">
-        <v>7.452066594657265e-20</v>
+        <v>7.452066594656948e-20</v>
       </c>
       <c r="F2">
-        <v>0.07199070804429436</v>
+        <v>0.07199070804429411</v>
       </c>
       <c r="G2">
         <v>0.01680416842176199</v>
@@ -1124,92 +1163,92 @@
         <v>6.661278729788306e-08</v>
       </c>
       <c r="I2">
-        <v>1.384164767812207e-07</v>
+        <v>1.384164767810545e-07</v>
       </c>
       <c r="J2">
-        <v>2.808434087000289e-07</v>
+        <v>2.808434086996897e-07</v>
       </c>
       <c r="K2">
-        <v>2.879574846677609e-10</v>
+        <v>2.879574846674172e-10</v>
       </c>
       <c r="L2">
-        <v>2.425187923593632e-11</v>
+        <v>2.425187923590737e-11</v>
       </c>
       <c r="M2">
-        <v>2.21702589109455e-10</v>
+        <v>2.217025891091896e-10</v>
       </c>
       <c r="N2">
         <v>5.71419026054514e-10</v>
       </c>
       <c r="O2">
-        <v>9.502124992473862e-06</v>
+        <v>9.50212499246245e-06</v>
       </c>
       <c r="P2">
-        <v>2.547933406246887e-20</v>
+        <v>2.547933406243737e-20</v>
       </c>
       <c r="Q2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3">
-        <v>3.926263634722557e-08</v>
+        <v>3.926263634722585e-08</v>
       </c>
       <c r="B3">
-        <v>6.393190443563186e-06</v>
+        <v>6.393190443563118e-06</v>
       </c>
       <c r="C3">
         <v>6.478803798340729e-05</v>
       </c>
       <c r="D3">
-        <v>3.403799932182848e-09</v>
+        <v>3.403799932182812e-09</v>
       </c>
       <c r="E3">
         <v>4.816083294337537e-20</v>
       </c>
       <c r="F3">
-        <v>0.07580486858508011</v>
+        <v>0.07580486858507984</v>
       </c>
       <c r="G3">
         <v>0.01269628190368889</v>
       </c>
       <c r="H3">
-        <v>3.611237190463062e-08</v>
+        <v>3.611237190463088e-08</v>
       </c>
       <c r="I3">
-        <v>4.588398451095249e-07</v>
+        <v>4.588398451095184e-07</v>
       </c>
       <c r="J3">
-        <v>9.802982417111789e-07</v>
+        <v>9.802982417111649e-07</v>
       </c>
       <c r="K3">
         <v>6.849211576790937e-10</v>
       </c>
       <c r="L3">
-        <v>4.358300176601331e-11</v>
+        <v>4.358300176601269e-11</v>
       </c>
       <c r="M3">
-        <v>9.727126586421368e-10</v>
+        <v>9.727126586421196e-10</v>
       </c>
       <c r="N3">
         <v>4.48223712219935e-10</v>
       </c>
       <c r="O3">
-        <v>1.840575689658404e-05</v>
+        <v>1.840575689658391e-05</v>
       </c>
       <c r="P3">
-        <v>5.183916705714027e-20</v>
+        <v>5.183916705713953e-20</v>
       </c>
       <c r="Q3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4">
-        <v>5.472287028230602e-08</v>
+        <v>5.472287028230582e-08</v>
       </c>
       <c r="B4">
-        <v>3.992919618799619e-06</v>
+        <v>3.992919618799648e-06</v>
       </c>
       <c r="C4">
         <v>4.810700239698601e-05</v>
@@ -1218,7 +1257,7 @@
         <v>8.971140220376964e-09</v>
       </c>
       <c r="E4">
-        <v>2.606254635998999e-20</v>
+        <v>2.60625463599898e-20</v>
       </c>
       <c r="F4">
         <v>0.06598715982023311</v>
@@ -1227,7 +1266,7 @@
         <v>0.01540381537647643</v>
       </c>
       <c r="H4">
-        <v>6.10656765883961e-08</v>
+        <v>6.106567658839566e-08</v>
       </c>
       <c r="I4">
         <v>1.052705958060885e-06</v>
@@ -1242,7 +1281,7 @@
         <v>1.690846777941747e-10</v>
       </c>
       <c r="M4">
-        <v>1.839410986935779e-09</v>
+        <v>1.839410986935786e-09</v>
       </c>
       <c r="N4">
         <v>3.328191417630642e-10</v>
@@ -1251,63 +1290,63 @@
         <v>2.674633239193673e-05</v>
       </c>
       <c r="P4">
-        <v>7.393745364001238e-20</v>
+        <v>7.393745364001132e-20</v>
       </c>
       <c r="Q4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>5.472794061560738e-08</v>
+        <v>5.472794061560855e-08</v>
       </c>
       <c r="B5">
-        <v>3.810716080097701e-06</v>
+        <v>3.810716080097586e-06</v>
       </c>
       <c r="C5">
-        <v>3.520489829357488e-05</v>
+        <v>3.520489829421788e-05</v>
       </c>
       <c r="D5">
-        <v>2.079209581070944e-08</v>
+        <v>2.079209580854643e-08</v>
       </c>
       <c r="E5">
-        <v>1.320125396748132e-20</v>
+        <v>1.320125396819626e-20</v>
       </c>
       <c r="F5">
-        <v>0.06298189140324958</v>
+        <v>0.06298189140324913</v>
       </c>
       <c r="G5">
-        <v>0.01470363810072552</v>
+        <v>0.01470363810072573</v>
       </c>
       <c r="H5">
-        <v>5.829534959538155e-08</v>
+        <v>5.829534959538362e-08</v>
       </c>
       <c r="I5">
-        <v>2.328702269840826e-06</v>
+        <v>2.328702269598553e-06</v>
       </c>
       <c r="J5">
-        <v>4.133611580623404e-06</v>
+        <v>4.133611580193353e-06</v>
       </c>
       <c r="K5">
-        <v>4.845326785254299e-09</v>
+        <v>4.84532678475034e-09</v>
       </c>
       <c r="L5">
-        <v>3.570654895631718e-10</v>
+        <v>3.570654895260388e-10</v>
       </c>
       <c r="M5">
-        <v>4.262743114543116e-09</v>
+        <v>4.262743114099569e-09</v>
       </c>
       <c r="N5">
-        <v>2.435583896754631e-10</v>
+        <v>2.435583896799107e-10</v>
       </c>
       <c r="O5">
-        <v>3.319742938003905e-05</v>
+        <v>3.319742937779818e-05</v>
       </c>
       <c r="P5">
-        <v>8.679874660303066e-20</v>
+        <v>8.679874659870236e-20</v>
       </c>
       <c r="Q5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1318,13 +1357,13 @@
         <v>3.628115830173329e-06</v>
       </c>
       <c r="C6">
-        <v>2.643535036864405e-05</v>
+        <v>2.643535036871176e-05</v>
       </c>
       <c r="D6">
-        <v>4.174576686516866e-08</v>
+        <v>4.174576686484816e-08</v>
       </c>
       <c r="E6">
-        <v>7.041673031468779e-21</v>
+        <v>7.041673031512358e-21</v>
       </c>
       <c r="F6">
         <v>0.05997334253839248</v>
@@ -1336,48 +1375,48 @@
         <v>5.552805679012911e-08</v>
       </c>
       <c r="I6">
-        <v>4.452159326695709e-06</v>
+        <v>4.452159326661512e-06</v>
       </c>
       <c r="J6">
-        <v>7.525388963257135e-06</v>
+        <v>7.525388963199386e-06</v>
       </c>
       <c r="K6">
-        <v>9.265050874299939e-09</v>
+        <v>9.265050874228841e-09</v>
       </c>
       <c r="L6">
-        <v>6.502542109907156e-10</v>
+        <v>6.502542109857164e-10</v>
       </c>
       <c r="M6">
-        <v>8.557271924899375e-09</v>
+        <v>8.557271924833677e-09</v>
       </c>
       <c r="N6">
-        <v>1.828879411212124e-10</v>
+        <v>1.828879411216808e-10</v>
       </c>
       <c r="O6">
-        <v>3.758223337444642e-05</v>
+        <v>3.758223337435055e-05</v>
       </c>
       <c r="P6">
-        <v>9.295832697271403e-20</v>
+        <v>9.295832697257532e-20</v>
       </c>
       <c r="Q6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>5.474828124361427e-08</v>
+        <v>5.474828124361447e-08</v>
       </c>
       <c r="B7">
-        <v>3.445226938358756e-06</v>
+        <v>3.445226938358738e-06</v>
       </c>
       <c r="C7">
-        <v>2.08363248078989e-05</v>
+        <v>2.083632480789901e-05</v>
       </c>
       <c r="D7">
-        <v>7.22009754521899e-08</v>
+        <v>7.220097545218914e-08</v>
       </c>
       <c r="E7">
-        <v>4.196047184234246e-21</v>
+        <v>4.196047184234306e-21</v>
       </c>
       <c r="F7">
         <v>0.05696240586654078</v>
@@ -1386,25 +1425,25 @@
         <v>0.01330328249663068</v>
       </c>
       <c r="H7">
-        <v>5.276297841589168e-08</v>
+        <v>5.276297841589205e-08</v>
       </c>
       <c r="I7">
-        <v>7.313603115110963e-06</v>
+        <v>7.313603115110911e-06</v>
       </c>
       <c r="J7">
-        <v>1.174139538222163e-05</v>
+        <v>1.174139538222146e-05</v>
       </c>
       <c r="K7">
-        <v>1.522305717455565e-08</v>
+        <v>1.522305717455544e-08</v>
       </c>
       <c r="L7">
-        <v>1.014987495810209e-09</v>
+        <v>1.014987495810195e-09</v>
       </c>
       <c r="M7">
-        <v>1.479696257778118e-08</v>
+        <v>1.479696257778097e-08</v>
       </c>
       <c r="N7">
-        <v>1.441521482223101e-10</v>
+        <v>1.441521482223106e-10</v>
       </c>
       <c r="O7">
         <v>4.038176551997847e-05</v>
@@ -1413,113 +1452,113 @@
         <v>9.580395281576764e-20</v>
       </c>
       <c r="Q7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>5.47626832629991e-08</v>
+        <v>5.476268326299871e-08</v>
       </c>
       <c r="B8">
-        <v>3.262181506338449e-06</v>
+        <v>3.262181506338478e-06</v>
       </c>
       <c r="C8">
-        <v>1.711762037283047e-05</v>
+        <v>1.711762037266456e-05</v>
       </c>
       <c r="D8">
-        <v>1.119048096652854e-07</v>
+        <v>1.119048096678588e-07</v>
       </c>
       <c r="E8">
-        <v>2.748203447666309e-21</v>
+        <v>2.748203447606947e-21</v>
       </c>
       <c r="F8">
         <v>0.05395017290376282</v>
       </c>
       <c r="G8">
-        <v>0.0126031051721783</v>
+        <v>0.01260310517217821</v>
       </c>
       <c r="H8">
-        <v>4.999911070942407e-08</v>
+        <v>4.999911070942336e-08</v>
       </c>
       <c r="I8">
-        <v>1.073597752781412e-05</v>
+        <v>1.073597752806097e-05</v>
       </c>
       <c r="J8">
-        <v>1.632429500948693e-05</v>
+        <v>1.632429500986251e-05</v>
       </c>
       <c r="K8">
-        <v>2.235251079684441e-08</v>
+        <v>2.235251079735837e-08</v>
       </c>
       <c r="L8">
-        <v>1.411899790425666e-09</v>
+        <v>1.411899790458131e-09</v>
       </c>
       <c r="M8">
-        <v>2.292788703698051e-08</v>
+        <v>2.292788703750794e-08</v>
       </c>
       <c r="N8">
-        <v>1.184249992235704e-10</v>
+        <v>1.184249992224227e-10</v>
       </c>
       <c r="O8">
-        <v>4.224113062521041e-05</v>
+        <v>4.224113062536318e-05</v>
       </c>
       <c r="P8">
-        <v>9.725179657886384e-20</v>
+        <v>9.725179657899928e-20</v>
       </c>
       <c r="Q8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9">
-        <v>5.477943844784317e-08</v>
+        <v>5.477943844784297e-08</v>
       </c>
       <c r="B9">
-        <v>3.07906377005466e-06</v>
+        <v>3.079063770054666e-06</v>
       </c>
       <c r="C9">
-        <v>1.447752824728145e-05</v>
+        <v>1.447752824728188e-05</v>
       </c>
       <c r="D9">
-        <v>1.61328409204417e-07</v>
+        <v>1.613284092044056e-07</v>
       </c>
       <c r="E9">
-        <v>1.922466080266764e-21</v>
+        <v>1.922466080266887e-21</v>
       </c>
       <c r="F9">
         <v>0.05093733972013908</v>
       </c>
       <c r="G9">
-        <v>0.01190292879117023</v>
+        <v>0.01190292879117014</v>
       </c>
       <c r="H9">
-        <v>4.723581482237107e-08</v>
+        <v>4.723581482237041e-08</v>
       </c>
       <c r="I9">
-        <v>1.461325998649199e-05</v>
+        <v>1.461325998649096e-05</v>
       </c>
       <c r="J9">
-        <v>2.097893176913461e-05</v>
+        <v>2.097893176913312e-05</v>
       </c>
       <c r="K9">
-        <v>3.043439597862113e-08</v>
+        <v>3.043439597861853e-08</v>
       </c>
       <c r="L9">
-        <v>1.815593094792928e-09</v>
+        <v>1.815593094792773e-09</v>
       </c>
       <c r="M9">
-        <v>3.304405036989956e-08</v>
+        <v>3.304405036989733e-08</v>
       </c>
       <c r="N9">
-        <v>1.001600242382301e-10</v>
+        <v>1.001600242382333e-10</v>
       </c>
       <c r="O9">
-        <v>4.356118579638431e-05</v>
+        <v>4.356118579638399e-05</v>
       </c>
       <c r="P9">
         <v>9.807753391976785e-20</v>
       </c>
       <c r="Q9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1527,37 +1566,37 @@
         <v>5.479856550316257e-08</v>
       </c>
       <c r="B10">
-        <v>2.895919008037259e-06</v>
+        <v>2.895919008037269e-06</v>
       </c>
       <c r="C10">
-        <v>1.248606345056472e-05</v>
+        <v>1.248606345056469e-05</v>
       </c>
       <c r="D10">
         <v>2.218524029222345e-07</v>
       </c>
       <c r="E10">
-        <v>1.405365041953481e-21</v>
+        <v>1.405365041953491e-21</v>
       </c>
       <c r="F10">
-        <v>0.04792428049144485</v>
+        <v>0.04792428049144502</v>
       </c>
       <c r="G10">
-        <v>0.01120275378640446</v>
+        <v>0.01120275378640454</v>
       </c>
       <c r="H10">
-        <v>4.447274957576346e-08</v>
+        <v>4.447274957576378e-08</v>
       </c>
       <c r="I10">
         <v>1.890687436451033e-05</v>
       </c>
       <c r="J10">
-        <v>2.553732124423323e-05</v>
+        <v>2.55373212442336e-05</v>
       </c>
       <c r="K10">
         <v>3.939026732318205e-08</v>
       </c>
       <c r="L10">
-        <v>2.211636350226684e-09</v>
+        <v>2.211636350226715e-09</v>
       </c>
       <c r="M10">
         <v>4.542500117007906e-08</v>
@@ -1569,116 +1608,116 @@
         <v>4.45569250834907e-05</v>
       </c>
       <c r="P10">
-        <v>9.85946349580465e-20</v>
+        <v>9.85946349580479e-20</v>
       </c>
       <c r="Q10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11">
-        <v>5.472288754799039e-08</v>
+        <v>5.472288754799019e-08</v>
       </c>
       <c r="B11">
-        <v>2.722439150827048e-06</v>
+        <v>2.722439150827058e-06</v>
       </c>
       <c r="C11">
-        <v>4.295780970943569e-05</v>
+        <v>4.29578097093822e-05</v>
       </c>
       <c r="D11">
-        <v>1.23337098223445e-08</v>
+        <v>1.233370982238411e-08</v>
       </c>
       <c r="E11">
-        <v>1.734601305261121e-05</v>
+        <v>1.734601305255485e-05</v>
       </c>
       <c r="F11">
         <v>0.04499115964694617</v>
       </c>
       <c r="G11">
-        <v>0.01050258470471671</v>
+        <v>0.01050258470471664</v>
       </c>
       <c r="H11">
-        <v>4.163563556158009e-08</v>
+        <v>4.16356355615795e-08</v>
       </c>
       <c r="I11">
-        <v>9.867813066528182e-07</v>
+        <v>9.867813066559874e-07</v>
       </c>
       <c r="J11">
-        <v>1.251261554704541e-06</v>
+        <v>1.25126155470856e-06</v>
       </c>
       <c r="K11">
-        <v>2.053004585266951e-09</v>
+        <v>2.053004585273515e-09</v>
       </c>
       <c r="L11">
-        <v>1.080652623676415e-10</v>
+        <v>1.08065262367987e-10</v>
       </c>
       <c r="M11">
-        <v>2.528859614460182e-09</v>
+        <v>2.528859614468313e-09</v>
       </c>
       <c r="N11">
-        <v>2.971954319982975e-10</v>
+        <v>2.971954319979268e-10</v>
       </c>
       <c r="O11">
-        <v>2.932094654821348e-05</v>
+        <v>2.932094654823452e-05</v>
       </c>
       <c r="P11">
-        <v>6.765398695385759e-05</v>
+        <v>6.765398695385519e-05</v>
       </c>
       <c r="Q11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <v>5.471940890247937e-08</v>
+        <v>5.471940890247956e-08</v>
       </c>
       <c r="B12">
-        <v>2.722785342797729e-06</v>
+        <v>2.722785342797715e-06</v>
       </c>
       <c r="C12">
-        <v>7.104717707840947e-05</v>
+        <v>7.104717707827014e-05</v>
       </c>
       <c r="D12">
-        <v>2.226178028206273e-09</v>
+        <v>2.22617802822111e-09</v>
       </c>
       <c r="E12">
-        <v>4.988323497784697e-05</v>
+        <v>4.988323497739195e-05</v>
       </c>
       <c r="F12">
-        <v>0.04499402045303071</v>
+        <v>0.04499402045303055</v>
       </c>
       <c r="G12">
         <v>0.01050258484686324</v>
       </c>
       <c r="H12">
-        <v>4.163298941500336e-08</v>
+        <v>4.163298941500366e-08</v>
       </c>
       <c r="I12">
-        <v>1.781208231482807e-07</v>
+        <v>1.781208231494679e-07</v>
       </c>
       <c r="J12">
-        <v>2.258756913643002e-07</v>
+        <v>2.258756913658024e-07</v>
       </c>
       <c r="K12">
-        <v>3.705579121948515e-10</v>
+        <v>3.705579121973265e-10</v>
       </c>
       <c r="L12">
-        <v>1.950528451475127e-11</v>
+        <v>1.950528451488155e-11</v>
       </c>
       <c r="M12">
-        <v>4.564765739082778e-10</v>
+        <v>4.564765739113185e-10</v>
       </c>
       <c r="N12">
-        <v>4.915263749920553e-10</v>
+        <v>4.915263749910913e-10</v>
       </c>
       <c r="O12">
-        <v>1.447616570023402e-05</v>
+        <v>1.447616570027372e-05</v>
       </c>
       <c r="P12">
-        <v>3.51167650716732e-05</v>
+        <v>3.511676507158699e-05</v>
       </c>
       <c r="Q12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1696,10 +1735,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1708,15 +1747,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>4.083045303377627</v>
@@ -1728,15 +1767,15 @@
         <v>0.0005624203012347578</v>
       </c>
       <c r="E2">
-        <v>18.70497045762571</v>
+        <v>18.70497045760325</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>4.188505171866399</v>
@@ -1748,15 +1787,15 @@
         <v>0.0004411650710826132</v>
       </c>
       <c r="E3">
-        <v>36.23180491453552</v>
+        <v>36.23180491453526</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>4.317791703646318</v>
@@ -1771,118 +1810,118 @@
         <v>52.65026061404868</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5">
-        <v>4.453396906014182</v>
+        <v>4.45339690600625</v>
       </c>
       <c r="C5">
-        <v>34.65049044643197</v>
+        <v>34.65049044706485</v>
       </c>
       <c r="D5">
-        <v>0.0002397228244837235</v>
+        <v>0.0002397228244881011</v>
       </c>
       <c r="E5">
-        <v>65.34927043314774</v>
+        <v>65.34927042873656</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>4.57781492917185</v>
+        <v>4.577814929170737</v>
       </c>
       <c r="C6">
-        <v>26.01904563842918</v>
+        <v>26.01904563849583</v>
       </c>
       <c r="D6">
-        <v>0.0001800078160641854</v>
+        <v>0.0001800078160646465</v>
       </c>
       <c r="E6">
-        <v>73.98077435914649</v>
+        <v>73.98077435895777</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7">
-        <v>4.681178881169332</v>
+        <v>4.68117888116933</v>
       </c>
       <c r="C7">
-        <v>20.50819370856191</v>
+        <v>20.50819370856202</v>
       </c>
       <c r="D7">
-        <v>0.00014188203565188</v>
+        <v>0.0001418820356518805</v>
       </c>
       <c r="E7">
         <v>79.49166440940645</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8">
-        <v>4.766556609447369</v>
+        <v>4.766556609451578</v>
       </c>
       <c r="C8">
-        <v>16.84805154806148</v>
+        <v>16.84805154789819</v>
       </c>
       <c r="D8">
-        <v>0.0001165600386058764</v>
+        <v>0.0001165600386047467</v>
       </c>
       <c r="E8">
-        <v>83.15183193939058</v>
+        <v>83.15183193969132</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>4.839305579036515</v>
+        <v>4.839305579036503</v>
       </c>
       <c r="C9">
-        <v>14.24953567645812</v>
+        <v>14.24953567645855</v>
       </c>
       <c r="D9">
-        <v>9.858270102188003e-05</v>
+        <v>9.858270102188319e-05</v>
       </c>
       <c r="E9">
-        <v>85.75036574091398</v>
+        <v>85.75036574091338</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10">
-        <v>4.90357446244012</v>
+        <v>4.903574462440121</v>
       </c>
       <c r="C10">
-        <v>12.28943253008338</v>
+        <v>12.28943253008336</v>
       </c>
       <c r="D10">
         <v>8.502210039330329e-05</v>
@@ -1891,47 +1930,47 @@
         <v>87.71048244781633</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11">
-        <v>4.366957870124041</v>
+        <v>4.366957870124582</v>
       </c>
       <c r="C11">
-        <v>42.28130876912962</v>
+        <v>42.28130876907697</v>
       </c>
       <c r="D11">
-        <v>0.0002925151889747022</v>
+        <v>0.0002925151889743375</v>
       </c>
       <c r="E11">
-        <v>57.71839871695568</v>
+        <v>57.71839871699709</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <v>4.148453173241441</v>
+        <v>4.148453173242292</v>
       </c>
       <c r="C12">
-        <v>71.04717707840948</v>
+        <v>71.04717707827014</v>
       </c>
       <c r="D12">
-        <v>0.0004915263749920553</v>
+        <v>0.0004915263749910913</v>
       </c>
       <c r="E12">
-        <v>28.95233140046804</v>
+        <v>28.95233140054745</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1964,47 +2003,47 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>3.191891195797325e-16</v>
+        <v>6.938893903907228e-17</v>
       </c>
       <c r="B2">
-        <v>3.191891195797325e-16</v>
+        <v>6.938893903907228e-17</v>
       </c>
       <c r="C2">
-        <v>5.983752447528967e-15</v>
+        <v>5.960929991798147e-15</v>
       </c>
       <c r="D2">
-        <v>3.124353870780951e-15</v>
+        <v>3.112434423147188e-15</v>
       </c>
       <c r="E2">
-        <v>9.04153090223108e-30</v>
+        <v>9.006852126169957e-30</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>1.387778780781446e-16</v>
+        <v>-1.249000902703301e-16</v>
       </c>
       <c r="B3">
-        <v>1.387778780781446e-16</v>
+        <v>-1.249000902703301e-16</v>
       </c>
       <c r="C3">
-        <v>2.875846262517801e-16</v>
+        <v>2.873271282358147e-16</v>
       </c>
       <c r="D3">
-        <v>1.550680157197393e-16</v>
+        <v>1.549155497892335e-16</v>
       </c>
       <c r="E3">
-        <v>5.156436684853776e-31</v>
+        <v>5.148973706319275e-31</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2021,50 +2060,50 @@
         <v>6.911788849595091e-19</v>
       </c>
       <c r="E4">
-        <v>2.371301244026784e-33</v>
+        <v>1.131483842327501e-33</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>2.935152121352758e-13</v>
+        <v>2.92377233535035e-13</v>
       </c>
       <c r="B5">
-        <v>2.936123566499305e-13</v>
+        <v>2.922662112325725e-13</v>
       </c>
       <c r="C5">
-        <v>6.120426702341947e-13</v>
+        <v>6.082039169172382e-13</v>
       </c>
       <c r="D5">
-        <v>4.617034429473324e-13</v>
+        <v>4.587870881811451e-13</v>
       </c>
       <c r="E5">
-        <v>5.705119801905738e-28</v>
+        <v>5.668986226512874e-28</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>1.03667074924374e-14</v>
+        <v>1.020017403874363e-14</v>
       </c>
       <c r="B6">
-        <v>1.031119634120614e-14</v>
+        <v>1.015854067532018e-14</v>
       </c>
       <c r="C6">
-        <v>5.478012791645948e-15</v>
+        <v>5.353980063113606e-15</v>
       </c>
       <c r="D6">
-        <v>8.274719071835884e-15</v>
+        <v>8.086440588320198e-15</v>
       </c>
       <c r="E6">
-        <v>4.182806875593113e-30</v>
+        <v>4.087690010464689e-30</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2075,116 +2114,116 @@
         <v>-2.775557561562891e-17</v>
       </c>
       <c r="C7">
-        <v>4.065758146820642e-18</v>
+        <v>4.174178364069192e-18</v>
       </c>
       <c r="D7">
-        <v>1.149254302834635e-17</v>
+        <v>1.127570259384925e-17</v>
       </c>
       <c r="E7">
-        <v>1.889818757929975e-33</v>
+        <v>1.950004068692076e-33</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>4.153066779366554e-13</v>
+        <v>4.161254674173165e-13</v>
       </c>
       <c r="B8">
-        <v>4.153344335122711e-13</v>
+        <v>4.16236489719779e-13</v>
       </c>
       <c r="C8">
-        <v>4.825052033266553e-14</v>
+        <v>4.83901520199545e-14</v>
       </c>
       <c r="D8">
-        <v>2.698010949852767e-13</v>
+        <v>2.705799451684088e-13</v>
       </c>
       <c r="E8">
-        <v>2.653015442935812e-29</v>
+        <v>2.660622866216141e-29</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>1.1518563880486e-15</v>
+        <v>9.992007221626409e-16</v>
       </c>
       <c r="B9">
-        <v>1.110223024625157e-15</v>
+        <v>1.02695629777827e-15</v>
       </c>
       <c r="C9">
-        <v>7.429495386956919e-17</v>
+        <v>7.410521848938423e-17</v>
       </c>
       <c r="D9">
-        <v>6.587341349478804e-16</v>
+        <v>6.558745517179498e-16</v>
       </c>
       <c r="E9">
-        <v>3.461859075036056e-32</v>
+        <v>3.473896137188477e-32</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>-1.387778780781446e-16</v>
+        <v>1.804112415015879e-16</v>
       </c>
       <c r="B10">
-        <v>-8.326672684688674e-17</v>
+        <v>1.734723475976807e-16</v>
       </c>
       <c r="C10">
-        <v>1.219727444046192e-19</v>
+        <v>9.486769009248164e-20</v>
       </c>
       <c r="D10">
-        <v>8.131516293641283e-20</v>
+        <v>4.472333961502706e-19</v>
       </c>
       <c r="E10">
-        <v>-1.203706215242022e-35</v>
+        <v>1.384262147528326e-33</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>4.996003610813204e-16</v>
+        <v>3.608224830031759e-16</v>
       </c>
       <c r="B11">
-        <v>4.510281037539698e-16</v>
+        <v>3.885780586188048e-16</v>
       </c>
       <c r="C11">
-        <v>1.294645814164941e-15</v>
+        <v>1.283234586299531e-15</v>
       </c>
       <c r="D11">
-        <v>2.712877123466073e-15</v>
+        <v>2.738762450334165e-15</v>
       </c>
       <c r="E11">
-        <v>6.468783841917514e-15</v>
+        <v>6.410033636695955e-15</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>5.828670879282072e-16</v>
+        <v>4.163336342344337e-16</v>
       </c>
       <c r="B12">
-        <v>4.996003610813204e-16</v>
+        <v>3.469446951953614e-16</v>
       </c>
       <c r="C12">
-        <v>5.252498739768963e-15</v>
+        <v>5.192583017211982e-15</v>
       </c>
       <c r="D12">
-        <v>4.21862387687752e-15</v>
+        <v>4.174828885372683e-15</v>
       </c>
       <c r="E12">
-        <v>4.952016173422752e-14</v>
+        <v>4.897894156224991e-14</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3D->2D done. Splitting main function started.
</commit_message>
<xml_diff>
--- a/output/concentrations/ds.5p.ser/big_ser_test_res.xlsx
+++ b/output/concentrations/ds.5p.ser/big_ser_test_res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
   <si>
     <t>H</t>
   </si>
@@ -37,7 +37,25 @@
     <t>DNA</t>
   </si>
   <si>
-    <t>prod_names</t>
+    <t>lg_k</t>
+  </si>
+  <si>
+    <t>tot</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ass</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
   <si>
     <t>H+PO4</t>
@@ -65,27 +83,6 @@
   </si>
   <si>
     <t>Cu+DNA</t>
-  </si>
-  <si>
-    <t>lg_k</t>
-  </si>
-  <si>
-    <t>tot</t>
-  </si>
-  <si>
-    <t>series</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>ass</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
   <si>
     <t>p(Hydr)</t>
@@ -482,13 +479,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,11 +501,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -524,11 +518,8 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,11 +535,8 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -564,11 +552,8 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -584,11 +569,8 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -604,11 +586,8 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2</v>
       </c>
@@ -624,11 +603,8 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>4</v>
       </c>
@@ -644,11 +620,8 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>-1</v>
       </c>
@@ -664,11 +637,8 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>0</v>
       </c>
@@ -684,11 +654,8 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>0</v>
       </c>
@@ -704,11 +671,8 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>0</v>
       </c>
@@ -723,9 +687,6 @@
       </c>
       <c r="E12">
         <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -816,19 +777,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -848,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -868,7 +829,7 @@
         <v>1e-19</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -888,7 +849,7 @@
         <v>1e-19</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -908,7 +869,7 @@
         <v>1e-19</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -928,7 +889,7 @@
         <v>1e-19</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -948,7 +909,7 @@
         <v>1e-19</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -968,7 +929,7 @@
         <v>1e-19</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -988,7 +949,7 @@
         <v>1e-19</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1008,7 +969,7 @@
         <v>1e-19</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1028,7 +989,7 @@
         <v>1e-19</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1048,7 +1009,7 @@
         <v>8.500000000000001e-05</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1068,7 +1029,7 @@
         <v>8.500000000000001e-05</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1101,25 +1062,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
@@ -1128,13 +1089,13 @@
         <v>2</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1148,10 +1109,10 @@
         <v>8.259517860200998e-05</v>
       </c>
       <c r="D2">
-        <v>1.081213216202099e-09</v>
+        <v>1.081213216203394e-09</v>
       </c>
       <c r="E2">
-        <v>7.452066594656948e-20</v>
+        <v>7.452066594657265e-20</v>
       </c>
       <c r="F2">
         <v>0.07199070804429411</v>
@@ -1163,45 +1124,45 @@
         <v>6.661278729788306e-08</v>
       </c>
       <c r="I2">
-        <v>1.384164767810545e-07</v>
+        <v>1.384164767812207e-07</v>
       </c>
       <c r="J2">
-        <v>2.808434086996897e-07</v>
+        <v>2.808434087000249e-07</v>
       </c>
       <c r="K2">
-        <v>2.879574846674172e-10</v>
+        <v>2.879574846677609e-10</v>
       </c>
       <c r="L2">
-        <v>2.425187923590737e-11</v>
+        <v>2.425187923593632e-11</v>
       </c>
       <c r="M2">
-        <v>2.217025891091896e-10</v>
+        <v>2.21702589109455e-10</v>
       </c>
       <c r="N2">
         <v>5.71419026054514e-10</v>
       </c>
       <c r="O2">
-        <v>9.50212499246245e-06</v>
+        <v>9.502124992473862e-06</v>
       </c>
       <c r="P2">
-        <v>2.547933406243737e-20</v>
+        <v>2.547933406246887e-20</v>
       </c>
       <c r="Q2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3">
-        <v>3.926263634722585e-08</v>
+        <v>3.926263634722571e-08</v>
       </c>
       <c r="B3">
-        <v>6.393190443563118e-06</v>
+        <v>6.393190443563141e-06</v>
       </c>
       <c r="C3">
         <v>6.478803798340729e-05</v>
       </c>
       <c r="D3">
-        <v>3.403799932182812e-09</v>
+        <v>3.403799932182848e-09</v>
       </c>
       <c r="E3">
         <v>4.816083294337537e-20</v>
@@ -1213,48 +1174,48 @@
         <v>0.01269628190368889</v>
       </c>
       <c r="H3">
-        <v>3.611237190463088e-08</v>
+        <v>3.611237190463062e-08</v>
       </c>
       <c r="I3">
-        <v>4.588398451095184e-07</v>
+        <v>4.588398451095249e-07</v>
       </c>
       <c r="J3">
-        <v>9.802982417111649e-07</v>
+        <v>9.802982417111789e-07</v>
       </c>
       <c r="K3">
         <v>6.849211576790937e-10</v>
       </c>
       <c r="L3">
-        <v>4.358300176601269e-11</v>
+        <v>4.358300176601331e-11</v>
       </c>
       <c r="M3">
-        <v>9.727126586421196e-10</v>
+        <v>9.727126586421335e-10</v>
       </c>
       <c r="N3">
         <v>4.48223712219935e-10</v>
       </c>
       <c r="O3">
-        <v>1.840575689658391e-05</v>
+        <v>1.840575689658404e-05</v>
       </c>
       <c r="P3">
-        <v>5.183916705713953e-20</v>
+        <v>5.183916705714027e-20</v>
       </c>
       <c r="Q3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4">
-        <v>5.472287028230582e-08</v>
+        <v>5.472287028230602e-08</v>
       </c>
       <c r="B4">
-        <v>3.992919618799648e-06</v>
+        <v>3.992919618799619e-06</v>
       </c>
       <c r="C4">
         <v>4.810700239698601e-05</v>
       </c>
       <c r="D4">
-        <v>8.971140220376964e-09</v>
+        <v>8.971140220376932e-09</v>
       </c>
       <c r="E4">
         <v>2.60625463599898e-20</v>
@@ -1266,10 +1227,10 @@
         <v>0.01540381537647643</v>
       </c>
       <c r="H4">
-        <v>6.106567658839566e-08</v>
+        <v>6.10656765883961e-08</v>
       </c>
       <c r="I4">
-        <v>1.052705958060885e-06</v>
+        <v>1.052705958060878e-06</v>
       </c>
       <c r="J4">
         <v>1.95779185358042e-06</v>
@@ -1281,7 +1242,7 @@
         <v>1.690846777941747e-10</v>
       </c>
       <c r="M4">
-        <v>1.839410986935786e-09</v>
+        <v>1.839410986935773e-09</v>
       </c>
       <c r="N4">
         <v>3.328191417630642e-10</v>
@@ -1293,60 +1254,60 @@
         <v>7.393745364001132e-20</v>
       </c>
       <c r="Q4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>5.472794061560855e-08</v>
+        <v>5.472794061560738e-08</v>
       </c>
       <c r="B5">
-        <v>3.810716080097586e-06</v>
+        <v>3.810716080097701e-06</v>
       </c>
       <c r="C5">
-        <v>3.520489829421788e-05</v>
+        <v>3.520489829357488e-05</v>
       </c>
       <c r="D5">
-        <v>2.079209580854643e-08</v>
+        <v>2.079209581070944e-08</v>
       </c>
       <c r="E5">
-        <v>1.320125396819626e-20</v>
+        <v>1.320125396748132e-20</v>
       </c>
       <c r="F5">
-        <v>0.06298189140324913</v>
+        <v>0.06298189140324958</v>
       </c>
       <c r="G5">
-        <v>0.01470363810072573</v>
+        <v>0.01470363810072552</v>
       </c>
       <c r="H5">
-        <v>5.829534959538362e-08</v>
+        <v>5.829534959538155e-08</v>
       </c>
       <c r="I5">
-        <v>2.328702269598553e-06</v>
+        <v>2.328702269840826e-06</v>
       </c>
       <c r="J5">
-        <v>4.133611580193353e-06</v>
+        <v>4.133611580623404e-06</v>
       </c>
       <c r="K5">
-        <v>4.84532678475034e-09</v>
+        <v>4.845326785254299e-09</v>
       </c>
       <c r="L5">
-        <v>3.570654895260388e-10</v>
+        <v>3.570654895631718e-10</v>
       </c>
       <c r="M5">
-        <v>4.262743114099569e-09</v>
+        <v>4.262743114543116e-09</v>
       </c>
       <c r="N5">
-        <v>2.435583896799107e-10</v>
+        <v>2.435583896754631e-10</v>
       </c>
       <c r="O5">
-        <v>3.319742937779818e-05</v>
+        <v>3.319742938003905e-05</v>
       </c>
       <c r="P5">
-        <v>8.679874659870236e-20</v>
+        <v>8.679874660303066e-20</v>
       </c>
       <c r="Q5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1354,19 +1315,19 @@
         <v>5.473651091467139e-08</v>
       </c>
       <c r="B6">
-        <v>3.628115830173329e-06</v>
+        <v>3.628115830173335e-06</v>
       </c>
       <c r="C6">
-        <v>2.643535036871176e-05</v>
+        <v>2.6435350368644e-05</v>
       </c>
       <c r="D6">
-        <v>4.174576686484816e-08</v>
+        <v>4.174576686516881e-08</v>
       </c>
       <c r="E6">
-        <v>7.041673031512358e-21</v>
+        <v>7.041673031468728e-21</v>
       </c>
       <c r="F6">
-        <v>0.05997334253839248</v>
+        <v>0.05997334253839269</v>
       </c>
       <c r="G6">
         <v>0.01400346031491835</v>
@@ -1375,137 +1336,137 @@
         <v>5.552805679012911e-08</v>
       </c>
       <c r="I6">
-        <v>4.452159326661512e-06</v>
+        <v>4.452159326695709e-06</v>
       </c>
       <c r="J6">
-        <v>7.525388963199386e-06</v>
+        <v>7.525388963257135e-06</v>
       </c>
       <c r="K6">
-        <v>9.265050874228841e-09</v>
+        <v>9.265050874300005e-09</v>
       </c>
       <c r="L6">
-        <v>6.502542109857164e-10</v>
+        <v>6.502542109907156e-10</v>
       </c>
       <c r="M6">
-        <v>8.557271924833677e-09</v>
+        <v>8.557271924899404e-09</v>
       </c>
       <c r="N6">
-        <v>1.828879411216808e-10</v>
+        <v>1.828879411212117e-10</v>
       </c>
       <c r="O6">
-        <v>3.758223337435055e-05</v>
+        <v>3.758223337444642e-05</v>
       </c>
       <c r="P6">
-        <v>9.295832697257532e-20</v>
+        <v>9.295832697271403e-20</v>
       </c>
       <c r="Q6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>5.474828124361447e-08</v>
+        <v>5.474828124361408e-08</v>
       </c>
       <c r="B7">
-        <v>3.445226938358738e-06</v>
+        <v>3.445226938358781e-06</v>
       </c>
       <c r="C7">
-        <v>2.083632480789901e-05</v>
+        <v>2.083632480789886e-05</v>
       </c>
       <c r="D7">
-        <v>7.220097545218914e-08</v>
+        <v>7.22009754521899e-08</v>
       </c>
       <c r="E7">
-        <v>4.196047184234306e-21</v>
+        <v>4.196047184234246e-21</v>
       </c>
       <c r="F7">
-        <v>0.05696240586654078</v>
+        <v>0.05696240586654119</v>
       </c>
       <c r="G7">
         <v>0.01330328249663068</v>
       </c>
       <c r="H7">
-        <v>5.276297841589205e-08</v>
+        <v>5.276297841589168e-08</v>
       </c>
       <c r="I7">
-        <v>7.313603115110911e-06</v>
+        <v>7.313603115111066e-06</v>
       </c>
       <c r="J7">
-        <v>1.174139538222146e-05</v>
+        <v>1.174139538222179e-05</v>
       </c>
       <c r="K7">
-        <v>1.522305717455544e-08</v>
+        <v>1.522305717455565e-08</v>
       </c>
       <c r="L7">
-        <v>1.014987495810195e-09</v>
+        <v>1.014987495810209e-09</v>
       </c>
       <c r="M7">
-        <v>1.479696257778097e-08</v>
+        <v>1.479696257778123e-08</v>
       </c>
       <c r="N7">
-        <v>1.441521482223106e-10</v>
+        <v>1.441521482223096e-10</v>
       </c>
       <c r="O7">
-        <v>4.038176551997847e-05</v>
+        <v>4.038176551997819e-05</v>
       </c>
       <c r="P7">
         <v>9.580395281576764e-20</v>
       </c>
       <c r="Q7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>5.476268326299871e-08</v>
+        <v>5.476268326299929e-08</v>
       </c>
       <c r="B8">
-        <v>3.262181506338478e-06</v>
+        <v>3.262181506338426e-06</v>
       </c>
       <c r="C8">
-        <v>1.711762037266456e-05</v>
+        <v>1.71176203728305e-05</v>
       </c>
       <c r="D8">
-        <v>1.119048096678588e-07</v>
+        <v>1.119048096652858e-07</v>
       </c>
       <c r="E8">
-        <v>2.748203447606947e-21</v>
+        <v>2.74820344766629e-21</v>
       </c>
       <c r="F8">
-        <v>0.05395017290376282</v>
+        <v>0.05395017290376244</v>
       </c>
       <c r="G8">
-        <v>0.01260310517217821</v>
+        <v>0.0126031051721783</v>
       </c>
       <c r="H8">
-        <v>4.999911070942336e-08</v>
+        <v>4.999911070942407e-08</v>
       </c>
       <c r="I8">
-        <v>1.073597752806097e-05</v>
+        <v>1.073597752781412e-05</v>
       </c>
       <c r="J8">
-        <v>1.632429500986251e-05</v>
+        <v>1.632429500948693e-05</v>
       </c>
       <c r="K8">
-        <v>2.235251079735837e-08</v>
+        <v>2.235251079684441e-08</v>
       </c>
       <c r="L8">
-        <v>1.411899790458131e-09</v>
+        <v>1.411899790425687e-09</v>
       </c>
       <c r="M8">
-        <v>2.292788703750794e-08</v>
+        <v>2.292788703698051e-08</v>
       </c>
       <c r="N8">
-        <v>1.184249992224227e-10</v>
+        <v>1.184249992235709e-10</v>
       </c>
       <c r="O8">
-        <v>4.224113062536318e-05</v>
+        <v>4.224113062521102e-05</v>
       </c>
       <c r="P8">
-        <v>9.725179657899928e-20</v>
+        <v>9.725179657886384e-20</v>
       </c>
       <c r="Q8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1513,52 +1474,52 @@
         <v>5.477943844784297e-08</v>
       </c>
       <c r="B9">
-        <v>3.079063770054666e-06</v>
+        <v>3.079063770054671e-06</v>
       </c>
       <c r="C9">
-        <v>1.447752824728188e-05</v>
+        <v>1.447752824728147e-05</v>
       </c>
       <c r="D9">
-        <v>1.613284092044056e-07</v>
+        <v>1.613284092044167e-07</v>
       </c>
       <c r="E9">
-        <v>1.922466080266887e-21</v>
+        <v>1.922466080266764e-21</v>
       </c>
       <c r="F9">
         <v>0.05093733972013908</v>
       </c>
       <c r="G9">
-        <v>0.01190292879117014</v>
+        <v>0.01190292879117023</v>
       </c>
       <c r="H9">
         <v>4.723581482237041e-08</v>
       </c>
       <c r="I9">
-        <v>1.461325998649096e-05</v>
+        <v>1.461325998649189e-05</v>
       </c>
       <c r="J9">
-        <v>2.097893176913312e-05</v>
+        <v>2.097893176913461e-05</v>
       </c>
       <c r="K9">
-        <v>3.043439597861853e-08</v>
+        <v>3.043439597862091e-08</v>
       </c>
       <c r="L9">
-        <v>1.815593094792773e-09</v>
+        <v>1.815593094792928e-09</v>
       </c>
       <c r="M9">
-        <v>3.304405036989733e-08</v>
+        <v>3.304405036989968e-08</v>
       </c>
       <c r="N9">
-        <v>1.001600242382333e-10</v>
+        <v>1.001600242382305e-10</v>
       </c>
       <c r="O9">
-        <v>4.356118579638399e-05</v>
+        <v>4.356118579638462e-05</v>
       </c>
       <c r="P9">
         <v>9.807753391976785e-20</v>
       </c>
       <c r="Q9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1566,16 +1527,16 @@
         <v>5.479856550316257e-08</v>
       </c>
       <c r="B10">
-        <v>2.895919008037269e-06</v>
+        <v>2.895919008037264e-06</v>
       </c>
       <c r="C10">
-        <v>1.248606345056469e-05</v>
+        <v>1.248606345056467e-05</v>
       </c>
       <c r="D10">
-        <v>2.218524029222345e-07</v>
+        <v>2.218524029222357e-07</v>
       </c>
       <c r="E10">
-        <v>1.405365041953491e-21</v>
+        <v>1.405365041953481e-21</v>
       </c>
       <c r="F10">
         <v>0.04792428049144502</v>
@@ -1587,31 +1548,31 @@
         <v>4.447274957576378e-08</v>
       </c>
       <c r="I10">
-        <v>1.890687436451033e-05</v>
+        <v>1.890687436451046e-05</v>
       </c>
       <c r="J10">
         <v>2.55373212442336e-05</v>
       </c>
       <c r="K10">
-        <v>3.939026732318205e-08</v>
+        <v>3.939026732318233e-08</v>
       </c>
       <c r="L10">
         <v>2.211636350226715e-09</v>
       </c>
       <c r="M10">
-        <v>4.542500117007906e-08</v>
+        <v>4.542500117007921e-08</v>
       </c>
       <c r="N10">
-        <v>8.638245399959615e-11</v>
+        <v>8.638245399959584e-11</v>
       </c>
       <c r="O10">
         <v>4.45569250834907e-05</v>
       </c>
       <c r="P10">
-        <v>9.85946349580479e-20</v>
+        <v>9.85946349580465e-20</v>
       </c>
       <c r="Q10" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1619,19 +1580,19 @@
         <v>5.472288754799019e-08</v>
       </c>
       <c r="B11">
-        <v>2.722439150827058e-06</v>
+        <v>2.722439150827053e-06</v>
       </c>
       <c r="C11">
-        <v>4.29578097093822e-05</v>
+        <v>4.295780970943577e-05</v>
       </c>
       <c r="D11">
-        <v>1.233370982238411e-08</v>
+        <v>1.233370982234454e-08</v>
       </c>
       <c r="E11">
-        <v>1.734601305255485e-05</v>
+        <v>1.734601305261118e-05</v>
       </c>
       <c r="F11">
-        <v>0.04499115964694617</v>
+        <v>0.04499115964694601</v>
       </c>
       <c r="G11">
         <v>0.01050258470471664</v>
@@ -1640,84 +1601,84 @@
         <v>4.16356355615795e-08</v>
       </c>
       <c r="I11">
-        <v>9.867813066559874e-07</v>
+        <v>9.867813066528182e-07</v>
       </c>
       <c r="J11">
-        <v>1.25126155470856e-06</v>
+        <v>1.251261554704541e-06</v>
       </c>
       <c r="K11">
-        <v>2.053004585273515e-09</v>
+        <v>2.053004585266921e-09</v>
       </c>
       <c r="L11">
-        <v>1.08065262367987e-10</v>
+        <v>1.080652623676399e-10</v>
       </c>
       <c r="M11">
-        <v>2.528859614468313e-09</v>
+        <v>2.5288596144602e-09</v>
       </c>
       <c r="N11">
-        <v>2.971954319979268e-10</v>
+        <v>2.971954319982985e-10</v>
       </c>
       <c r="O11">
-        <v>2.932094654823452e-05</v>
+        <v>2.932094654821369e-05</v>
       </c>
       <c r="P11">
-        <v>6.765398695385519e-05</v>
+        <v>6.765398695385759e-05</v>
       </c>
       <c r="Q11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <v>5.471940890247956e-08</v>
+        <v>5.471940890247937e-08</v>
       </c>
       <c r="B12">
-        <v>2.722785342797715e-06</v>
+        <v>2.722785342797729e-06</v>
       </c>
       <c r="C12">
-        <v>7.104717707827014e-05</v>
+        <v>7.104717707840947e-05</v>
       </c>
       <c r="D12">
-        <v>2.22617802822111e-09</v>
+        <v>2.226178028206273e-09</v>
       </c>
       <c r="E12">
-        <v>4.988323497739195e-05</v>
+        <v>4.988323497784697e-05</v>
       </c>
       <c r="F12">
-        <v>0.04499402045303055</v>
+        <v>0.04499402045303071</v>
       </c>
       <c r="G12">
         <v>0.01050258484686324</v>
       </c>
       <c r="H12">
-        <v>4.163298941500366e-08</v>
+        <v>4.163298941500336e-08</v>
       </c>
       <c r="I12">
-        <v>1.781208231494679e-07</v>
+        <v>1.781208231482807e-07</v>
       </c>
       <c r="J12">
-        <v>2.258756913658024e-07</v>
+        <v>2.258756913643002e-07</v>
       </c>
       <c r="K12">
-        <v>3.705579121973265e-10</v>
+        <v>3.705579121948515e-10</v>
       </c>
       <c r="L12">
-        <v>1.950528451488155e-11</v>
+        <v>1.950528451475127e-11</v>
       </c>
       <c r="M12">
-        <v>4.564765739113185e-10</v>
+        <v>4.564765739082778e-10</v>
       </c>
       <c r="N12">
-        <v>4.915263749910913e-10</v>
+        <v>4.915263749920553e-10</v>
       </c>
       <c r="O12">
-        <v>1.447616570027372e-05</v>
+        <v>1.447616570023402e-05</v>
       </c>
       <c r="P12">
-        <v>3.511676507158699e-05</v>
+        <v>3.51167650716732e-05</v>
       </c>
       <c r="Q12" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1735,10 +1696,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1747,15 +1708,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>4.083045303377627</v>
@@ -1767,15 +1728,15 @@
         <v>0.0005624203012347578</v>
       </c>
       <c r="E2">
-        <v>18.70497045760325</v>
+        <v>18.70497045762571</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>4.188505171866399</v>
@@ -1787,15 +1748,15 @@
         <v>0.0004411650710826132</v>
       </c>
       <c r="E3">
-        <v>36.23180491453526</v>
+        <v>36.23180491453552</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>4.317791703646318</v>
@@ -1810,167 +1771,167 @@
         <v>52.65026061404868</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>4.45339690600625</v>
+        <v>4.453396906014182</v>
       </c>
       <c r="C5">
-        <v>34.65049044706485</v>
+        <v>34.65049044643197</v>
       </c>
       <c r="D5">
-        <v>0.0002397228244881011</v>
+        <v>0.0002397228244837235</v>
       </c>
       <c r="E5">
-        <v>65.34927042873656</v>
+        <v>65.34927043314774</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
-        <v>4.577814929170737</v>
+        <v>4.577814929171851</v>
       </c>
       <c r="C6">
-        <v>26.01904563849583</v>
+        <v>26.01904563842913</v>
       </c>
       <c r="D6">
-        <v>0.0001800078160646465</v>
+        <v>0.0001800078160641847</v>
       </c>
       <c r="E6">
-        <v>73.98077435895777</v>
+        <v>73.98077435914649</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
-        <v>4.68117888116933</v>
+        <v>4.681178881169333</v>
       </c>
       <c r="C7">
-        <v>20.50819370856202</v>
+        <v>20.50819370856187</v>
       </c>
       <c r="D7">
-        <v>0.0001418820356518805</v>
+        <v>0.0001418820356518795</v>
       </c>
       <c r="E7">
-        <v>79.49166440940645</v>
+        <v>79.49166440940589</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
-        <v>4.766556609451578</v>
+        <v>4.766556609447368</v>
       </c>
       <c r="C8">
-        <v>16.84805154789819</v>
+        <v>16.84805154806151</v>
       </c>
       <c r="D8">
-        <v>0.0001165600386047467</v>
+        <v>0.0001165600386058768</v>
       </c>
       <c r="E8">
-        <v>83.15183193969132</v>
+        <v>83.15183193939177</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>4.839305579036503</v>
+        <v>4.839305579036515</v>
       </c>
       <c r="C9">
-        <v>14.24953567645855</v>
+        <v>14.24953567645814</v>
       </c>
       <c r="D9">
-        <v>9.858270102188319e-05</v>
+        <v>9.858270102188038e-05</v>
       </c>
       <c r="E9">
-        <v>85.75036574091338</v>
+        <v>85.75036574091459</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>4.903574462440121</v>
       </c>
       <c r="C10">
-        <v>12.28943253008336</v>
+        <v>12.28943253008334</v>
       </c>
       <c r="D10">
-        <v>8.502210039330329e-05</v>
+        <v>8.502210039330299e-05</v>
       </c>
       <c r="E10">
         <v>87.71048244781633</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11">
-        <v>4.366957870124582</v>
+        <v>4.366957870124041</v>
       </c>
       <c r="C11">
-        <v>42.28130876907697</v>
+        <v>42.28130876912969</v>
       </c>
       <c r="D11">
-        <v>0.0002925151889743375</v>
+        <v>0.0002925151889747032</v>
       </c>
       <c r="E11">
-        <v>57.71839871699709</v>
+        <v>57.71839871695607</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
-        <v>4.148453173242292</v>
+        <v>4.148453173241441</v>
       </c>
       <c r="C12">
-        <v>71.04717707827014</v>
+        <v>71.04717707840948</v>
       </c>
       <c r="D12">
-        <v>0.0004915263749910913</v>
+        <v>0.0004915263749920553</v>
       </c>
       <c r="E12">
-        <v>28.95233140054745</v>
+        <v>28.95233140046804</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +1964,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2014,16 +1975,16 @@
         <v>6.938893903907228e-17</v>
       </c>
       <c r="C2">
-        <v>5.960929991798147e-15</v>
+        <v>5.983752447528967e-15</v>
       </c>
       <c r="D2">
-        <v>3.112434423147188e-15</v>
+        <v>3.124348788583267e-15</v>
       </c>
       <c r="E2">
-        <v>9.006852126169957e-30</v>
+        <v>9.04153090223108e-30</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2034,16 +1995,16 @@
         <v>-1.249000902703301e-16</v>
       </c>
       <c r="C3">
-        <v>2.873271282358147e-16</v>
+        <v>2.875846262517801e-16</v>
       </c>
       <c r="D3">
-        <v>1.549155497892335e-16</v>
+        <v>1.550680157197393e-16</v>
       </c>
       <c r="E3">
-        <v>5.148973706319275e-31</v>
+        <v>5.156436684853776e-31</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2057,113 +2018,113 @@
         <v>1.219727444046192e-18</v>
       </c>
       <c r="D4">
-        <v>6.911788849595091e-19</v>
+        <v>6.844026213814747e-19</v>
       </c>
       <c r="E4">
         <v>1.131483842327501e-33</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>2.92377233535035e-13</v>
+        <v>2.935152121352758e-13</v>
       </c>
       <c r="B5">
-        <v>2.922662112325725e-13</v>
+        <v>2.936123566499305e-13</v>
       </c>
       <c r="C5">
-        <v>6.082039169172382e-13</v>
+        <v>6.120426702341947e-13</v>
       </c>
       <c r="D5">
-        <v>4.587870881811451e-13</v>
+        <v>4.617034429473324e-13</v>
       </c>
       <c r="E5">
-        <v>5.668986226512874e-28</v>
+        <v>5.705119801905738e-28</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>1.020017403874363e-14</v>
+        <v>1.057487430955462e-14</v>
       </c>
       <c r="B6">
-        <v>1.015854067532018e-14</v>
+        <v>1.051936315832336e-14</v>
       </c>
       <c r="C6">
-        <v>5.353980063113606e-15</v>
+        <v>5.477958581537323e-15</v>
       </c>
       <c r="D6">
-        <v>8.086440588320198e-15</v>
+        <v>8.274719071835884e-15</v>
       </c>
       <c r="E6">
-        <v>4.087690010464689e-30</v>
+        <v>4.182758727344504e-30</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>-2.775557561562891e-17</v>
+        <v>3.747002708109903e-16</v>
       </c>
       <c r="B7">
-        <v>-2.775557561562891e-17</v>
+        <v>3.747002708109903e-16</v>
       </c>
       <c r="C7">
-        <v>4.174178364069192e-18</v>
+        <v>3.455894424797545e-18</v>
       </c>
       <c r="D7">
-        <v>1.127570259384925e-17</v>
+        <v>1.147899050119028e-17</v>
       </c>
       <c r="E7">
-        <v>1.950004068692076e-33</v>
+        <v>1.889818757929975e-33</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>4.161254674173165e-13</v>
+        <v>4.149180998780366e-13</v>
       </c>
       <c r="B8">
-        <v>4.16236489719779e-13</v>
+        <v>4.149597332414601e-13</v>
       </c>
       <c r="C8">
-        <v>4.83901520199545e-14</v>
+        <v>4.825175361263673e-14</v>
       </c>
       <c r="D8">
-        <v>2.705799451684088e-13</v>
+        <v>2.698016912964715e-13</v>
       </c>
       <c r="E8">
-        <v>2.660622866216141e-29</v>
+        <v>2.653013035523381e-29</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>9.992007221626409e-16</v>
+        <v>1.1518563880486e-15</v>
       </c>
       <c r="B9">
-        <v>1.02695629777827e-15</v>
+        <v>1.110223024625157e-15</v>
       </c>
       <c r="C9">
-        <v>7.410521848938423e-17</v>
+        <v>7.494547517306049e-17</v>
       </c>
       <c r="D9">
-        <v>6.558745517179498e-16</v>
+        <v>6.589374228552214e-16</v>
       </c>
       <c r="E9">
-        <v>3.473896137188477e-32</v>
+        <v>3.461859075036056e-32</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2174,56 +2135,56 @@
         <v>1.734723475976807e-16</v>
       </c>
       <c r="C10">
-        <v>9.486769009248164e-20</v>
+        <v>8.131516293641283e-20</v>
       </c>
       <c r="D10">
-        <v>4.472333961502706e-19</v>
+        <v>5.827586677109586e-19</v>
       </c>
       <c r="E10">
-        <v>1.384262147528326e-33</v>
+        <v>-1.203706215242022e-35</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>3.608224830031759e-16</v>
+        <v>1.942890293094024e-16</v>
       </c>
       <c r="B11">
-        <v>3.885780586188048e-16</v>
+        <v>2.220446049250313e-16</v>
       </c>
       <c r="C11">
-        <v>1.283234586299531e-15</v>
+        <v>1.295133705142559e-15</v>
       </c>
       <c r="D11">
-        <v>2.738762450334165e-15</v>
+        <v>2.713066858846258e-15</v>
       </c>
       <c r="E11">
-        <v>6.410033636695955e-15</v>
+        <v>6.468756736863202e-15</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>4.163336342344337e-16</v>
+        <v>5.828670879282072e-16</v>
       </c>
       <c r="B12">
-        <v>3.469446951953614e-16</v>
+        <v>4.996003610813204e-16</v>
       </c>
       <c r="C12">
-        <v>5.192583017211982e-15</v>
+        <v>5.252498739768963e-15</v>
       </c>
       <c r="D12">
-        <v>4.174828885372683e-15</v>
+        <v>4.21862387687752e-15</v>
       </c>
       <c r="E12">
-        <v>4.897894156224991e-14</v>
+        <v>4.952016173422752e-14</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
input equivalent concentrations python
</commit_message>
<xml_diff>
--- a/output/concentrations/ds.5p.ser/big_ser_test_res.xlsx
+++ b/output/concentrations/ds.5p.ser/big_ser_test_res.xlsx
@@ -11,16 +11,15 @@
     <sheet name="input_k_constants_log10" sheetId="2" r:id="rId2"/>
     <sheet name="input_concentrations" sheetId="3" r:id="rId3"/>
     <sheet name="equilibrium_concentrations" sheetId="4" r:id="rId4"/>
-    <sheet name="Hydr_fractions" sheetId="5" r:id="rId5"/>
-    <sheet name="percent_error" sheetId="6" r:id="rId6"/>
-    <sheet name="component_names" sheetId="7" r:id="rId7"/>
+    <sheet name="percent_error" sheetId="5" r:id="rId5"/>
+    <sheet name="component_names" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
   <si>
     <t>H</t>
   </si>
@@ -83,45 +82,6 @@
   </si>
   <si>
     <t>Cu+DNA</t>
-  </si>
-  <si>
-    <t>p(Hydr)</t>
-  </si>
-  <si>
-    <t>rn</t>
-  </si>
-  <si>
-    <t>S_1</t>
-  </si>
-  <si>
-    <t>S_2</t>
-  </si>
-  <si>
-    <t>S_3</t>
-  </si>
-  <si>
-    <t>S_4</t>
-  </si>
-  <si>
-    <t>S_5</t>
-  </si>
-  <si>
-    <t>S_6</t>
-  </si>
-  <si>
-    <t>S_7</t>
-  </si>
-  <si>
-    <t>S_8</t>
-  </si>
-  <si>
-    <t>S_9</t>
-  </si>
-  <si>
-    <t>S_10</t>
-  </si>
-  <si>
-    <t>S_11</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1069,10 @@
         <v>8.259517860200998e-05</v>
       </c>
       <c r="D2">
-        <v>1.081213216203394e-09</v>
+        <v>1.081213216202099e-09</v>
       </c>
       <c r="E2">
-        <v>7.452066594657265e-20</v>
+        <v>7.452066594656948e-20</v>
       </c>
       <c r="F2">
         <v>0.07199070804429411</v>
@@ -1124,28 +1084,28 @@
         <v>6.661278729788306e-08</v>
       </c>
       <c r="I2">
-        <v>1.384164767812207e-07</v>
+        <v>1.384164767810545e-07</v>
       </c>
       <c r="J2">
-        <v>2.808434087000249e-07</v>
+        <v>2.808434086996897e-07</v>
       </c>
       <c r="K2">
-        <v>2.879574846677609e-10</v>
+        <v>2.879574846674172e-10</v>
       </c>
       <c r="L2">
-        <v>2.425187923593632e-11</v>
+        <v>2.425187923590737e-11</v>
       </c>
       <c r="M2">
-        <v>2.21702589109455e-10</v>
+        <v>2.217025891091896e-10</v>
       </c>
       <c r="N2">
         <v>5.71419026054514e-10</v>
       </c>
       <c r="O2">
-        <v>9.502124992473862e-06</v>
+        <v>9.50212499246245e-06</v>
       </c>
       <c r="P2">
-        <v>2.547933406246887e-20</v>
+        <v>2.547933406243737e-20</v>
       </c>
       <c r="Q2" t="s">
         <v>8</v>
@@ -1153,16 +1113,16 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3">
-        <v>3.926263634722571e-08</v>
+        <v>3.926263634722585e-08</v>
       </c>
       <c r="B3">
-        <v>6.393190443563141e-06</v>
+        <v>6.393190443563118e-06</v>
       </c>
       <c r="C3">
         <v>6.478803798340729e-05</v>
       </c>
       <c r="D3">
-        <v>3.403799932182848e-09</v>
+        <v>3.403799932182812e-09</v>
       </c>
       <c r="E3">
         <v>4.816083294337537e-20</v>
@@ -1174,31 +1134,31 @@
         <v>0.01269628190368889</v>
       </c>
       <c r="H3">
-        <v>3.611237190463062e-08</v>
+        <v>3.611237190463088e-08</v>
       </c>
       <c r="I3">
-        <v>4.588398451095249e-07</v>
+        <v>4.588398451095184e-07</v>
       </c>
       <c r="J3">
-        <v>9.802982417111789e-07</v>
+        <v>9.802982417111649e-07</v>
       </c>
       <c r="K3">
         <v>6.849211576790937e-10</v>
       </c>
       <c r="L3">
-        <v>4.358300176601331e-11</v>
+        <v>4.358300176601269e-11</v>
       </c>
       <c r="M3">
-        <v>9.727126586421335e-10</v>
+        <v>9.727126586421196e-10</v>
       </c>
       <c r="N3">
         <v>4.48223712219935e-10</v>
       </c>
       <c r="O3">
-        <v>1.840575689658404e-05</v>
+        <v>1.840575689658391e-05</v>
       </c>
       <c r="P3">
-        <v>5.183916705714027e-20</v>
+        <v>5.183916705713953e-20</v>
       </c>
       <c r="Q3" t="s">
         <v>8</v>
@@ -1206,16 +1166,16 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4">
-        <v>5.472287028230602e-08</v>
+        <v>5.472287028230582e-08</v>
       </c>
       <c r="B4">
-        <v>3.992919618799619e-06</v>
+        <v>3.992919618799648e-06</v>
       </c>
       <c r="C4">
         <v>4.810700239698601e-05</v>
       </c>
       <c r="D4">
-        <v>8.971140220376932e-09</v>
+        <v>8.971140220376964e-09</v>
       </c>
       <c r="E4">
         <v>2.60625463599898e-20</v>
@@ -1227,10 +1187,10 @@
         <v>0.01540381537647643</v>
       </c>
       <c r="H4">
-        <v>6.10656765883961e-08</v>
+        <v>6.106567658839566e-08</v>
       </c>
       <c r="I4">
-        <v>1.052705958060878e-06</v>
+        <v>1.052705958060885e-06</v>
       </c>
       <c r="J4">
         <v>1.95779185358042e-06</v>
@@ -1242,7 +1202,7 @@
         <v>1.690846777941747e-10</v>
       </c>
       <c r="M4">
-        <v>1.839410986935773e-09</v>
+        <v>1.839410986935786e-09</v>
       </c>
       <c r="N4">
         <v>3.328191417630642e-10</v>
@@ -1259,52 +1219,52 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>5.472794061560738e-08</v>
+        <v>5.472794061560855e-08</v>
       </c>
       <c r="B5">
-        <v>3.810716080097701e-06</v>
+        <v>3.810716080097586e-06</v>
       </c>
       <c r="C5">
-        <v>3.520489829357488e-05</v>
+        <v>3.520489829421788e-05</v>
       </c>
       <c r="D5">
-        <v>2.079209581070944e-08</v>
+        <v>2.079209580854643e-08</v>
       </c>
       <c r="E5">
-        <v>1.320125396748132e-20</v>
+        <v>1.320125396819626e-20</v>
       </c>
       <c r="F5">
-        <v>0.06298189140324958</v>
+        <v>0.06298189140324913</v>
       </c>
       <c r="G5">
-        <v>0.01470363810072552</v>
+        <v>0.01470363810072573</v>
       </c>
       <c r="H5">
-        <v>5.829534959538155e-08</v>
+        <v>5.829534959538362e-08</v>
       </c>
       <c r="I5">
-        <v>2.328702269840826e-06</v>
+        <v>2.328702269598553e-06</v>
       </c>
       <c r="J5">
-        <v>4.133611580623404e-06</v>
+        <v>4.133611580193353e-06</v>
       </c>
       <c r="K5">
-        <v>4.845326785254299e-09</v>
+        <v>4.84532678475034e-09</v>
       </c>
       <c r="L5">
-        <v>3.570654895631718e-10</v>
+        <v>3.570654895260388e-10</v>
       </c>
       <c r="M5">
-        <v>4.262743114543116e-09</v>
+        <v>4.262743114099569e-09</v>
       </c>
       <c r="N5">
-        <v>2.435583896754631e-10</v>
+        <v>2.435583896799107e-10</v>
       </c>
       <c r="O5">
-        <v>3.319742938003905e-05</v>
+        <v>3.319742937779818e-05</v>
       </c>
       <c r="P5">
-        <v>8.679874660303066e-20</v>
+        <v>8.679874659870236e-20</v>
       </c>
       <c r="Q5" t="s">
         <v>9</v>
@@ -1315,19 +1275,19 @@
         <v>5.473651091467139e-08</v>
       </c>
       <c r="B6">
-        <v>3.628115830173335e-06</v>
+        <v>3.628115830173329e-06</v>
       </c>
       <c r="C6">
-        <v>2.6435350368644e-05</v>
+        <v>2.643535036871176e-05</v>
       </c>
       <c r="D6">
-        <v>4.174576686516881e-08</v>
+        <v>4.174576686484816e-08</v>
       </c>
       <c r="E6">
-        <v>7.041673031468728e-21</v>
+        <v>7.041673031512358e-21</v>
       </c>
       <c r="F6">
-        <v>0.05997334253839269</v>
+        <v>0.05997334253839248</v>
       </c>
       <c r="G6">
         <v>0.01400346031491835</v>
@@ -1336,28 +1296,28 @@
         <v>5.552805679012911e-08</v>
       </c>
       <c r="I6">
-        <v>4.452159326695709e-06</v>
+        <v>4.452159326661512e-06</v>
       </c>
       <c r="J6">
-        <v>7.525388963257135e-06</v>
+        <v>7.525388963199386e-06</v>
       </c>
       <c r="K6">
-        <v>9.265050874300005e-09</v>
+        <v>9.265050874228841e-09</v>
       </c>
       <c r="L6">
-        <v>6.502542109907156e-10</v>
+        <v>6.502542109857164e-10</v>
       </c>
       <c r="M6">
-        <v>8.557271924899404e-09</v>
+        <v>8.557271924833677e-09</v>
       </c>
       <c r="N6">
-        <v>1.828879411212117e-10</v>
+        <v>1.828879411216808e-10</v>
       </c>
       <c r="O6">
-        <v>3.758223337444642e-05</v>
+        <v>3.758223337435055e-05</v>
       </c>
       <c r="P6">
-        <v>9.295832697271403e-20</v>
+        <v>9.295832697257532e-20</v>
       </c>
       <c r="Q6" t="s">
         <v>10</v>
@@ -1365,49 +1325,49 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>5.474828124361408e-08</v>
+        <v>5.474828124361447e-08</v>
       </c>
       <c r="B7">
-        <v>3.445226938358781e-06</v>
+        <v>3.445226938358738e-06</v>
       </c>
       <c r="C7">
-        <v>2.083632480789886e-05</v>
+        <v>2.083632480789901e-05</v>
       </c>
       <c r="D7">
-        <v>7.22009754521899e-08</v>
+        <v>7.220097545218914e-08</v>
       </c>
       <c r="E7">
-        <v>4.196047184234246e-21</v>
+        <v>4.196047184234306e-21</v>
       </c>
       <c r="F7">
-        <v>0.05696240586654119</v>
+        <v>0.05696240586654078</v>
       </c>
       <c r="G7">
         <v>0.01330328249663068</v>
       </c>
       <c r="H7">
-        <v>5.276297841589168e-08</v>
+        <v>5.276297841589205e-08</v>
       </c>
       <c r="I7">
-        <v>7.313603115111066e-06</v>
+        <v>7.313603115110911e-06</v>
       </c>
       <c r="J7">
-        <v>1.174139538222179e-05</v>
+        <v>1.174139538222146e-05</v>
       </c>
       <c r="K7">
-        <v>1.522305717455565e-08</v>
+        <v>1.522305717455544e-08</v>
       </c>
       <c r="L7">
-        <v>1.014987495810209e-09</v>
+        <v>1.014987495810195e-09</v>
       </c>
       <c r="M7">
-        <v>1.479696257778123e-08</v>
+        <v>1.479696257778097e-08</v>
       </c>
       <c r="N7">
-        <v>1.441521482223096e-10</v>
+        <v>1.441521482223106e-10</v>
       </c>
       <c r="O7">
-        <v>4.038176551997819e-05</v>
+        <v>4.038176551997847e-05</v>
       </c>
       <c r="P7">
         <v>9.580395281576764e-20</v>
@@ -1418,52 +1378,52 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>5.476268326299929e-08</v>
+        <v>5.476268326299871e-08</v>
       </c>
       <c r="B8">
-        <v>3.262181506338426e-06</v>
+        <v>3.262181506338478e-06</v>
       </c>
       <c r="C8">
-        <v>1.71176203728305e-05</v>
+        <v>1.711762037266456e-05</v>
       </c>
       <c r="D8">
-        <v>1.119048096652858e-07</v>
+        <v>1.119048096678588e-07</v>
       </c>
       <c r="E8">
-        <v>2.74820344766629e-21</v>
+        <v>2.748203447606947e-21</v>
       </c>
       <c r="F8">
-        <v>0.05395017290376244</v>
+        <v>0.05395017290376282</v>
       </c>
       <c r="G8">
-        <v>0.0126031051721783</v>
+        <v>0.01260310517217821</v>
       </c>
       <c r="H8">
-        <v>4.999911070942407e-08</v>
+        <v>4.999911070942336e-08</v>
       </c>
       <c r="I8">
-        <v>1.073597752781412e-05</v>
+        <v>1.073597752806097e-05</v>
       </c>
       <c r="J8">
-        <v>1.632429500948693e-05</v>
+        <v>1.632429500986251e-05</v>
       </c>
       <c r="K8">
-        <v>2.235251079684441e-08</v>
+        <v>2.235251079735837e-08</v>
       </c>
       <c r="L8">
-        <v>1.411899790425687e-09</v>
+        <v>1.411899790458131e-09</v>
       </c>
       <c r="M8">
-        <v>2.292788703698051e-08</v>
+        <v>2.292788703750794e-08</v>
       </c>
       <c r="N8">
-        <v>1.184249992235709e-10</v>
+        <v>1.184249992224227e-10</v>
       </c>
       <c r="O8">
-        <v>4.224113062521102e-05</v>
+        <v>4.224113062536318e-05</v>
       </c>
       <c r="P8">
-        <v>9.725179657886384e-20</v>
+        <v>9.725179657899928e-20</v>
       </c>
       <c r="Q8" t="s">
         <v>10</v>
@@ -1474,46 +1434,46 @@
         <v>5.477943844784297e-08</v>
       </c>
       <c r="B9">
-        <v>3.079063770054671e-06</v>
+        <v>3.079063770054666e-06</v>
       </c>
       <c r="C9">
-        <v>1.447752824728147e-05</v>
+        <v>1.447752824728188e-05</v>
       </c>
       <c r="D9">
-        <v>1.613284092044167e-07</v>
+        <v>1.613284092044056e-07</v>
       </c>
       <c r="E9">
-        <v>1.922466080266764e-21</v>
+        <v>1.922466080266887e-21</v>
       </c>
       <c r="F9">
         <v>0.05093733972013908</v>
       </c>
       <c r="G9">
-        <v>0.01190292879117023</v>
+        <v>0.01190292879117014</v>
       </c>
       <c r="H9">
         <v>4.723581482237041e-08</v>
       </c>
       <c r="I9">
-        <v>1.461325998649189e-05</v>
+        <v>1.461325998649096e-05</v>
       </c>
       <c r="J9">
-        <v>2.097893176913461e-05</v>
+        <v>2.097893176913312e-05</v>
       </c>
       <c r="K9">
-        <v>3.043439597862091e-08</v>
+        <v>3.043439597861853e-08</v>
       </c>
       <c r="L9">
-        <v>1.815593094792928e-09</v>
+        <v>1.815593094792773e-09</v>
       </c>
       <c r="M9">
-        <v>3.304405036989968e-08</v>
+        <v>3.304405036989733e-08</v>
       </c>
       <c r="N9">
-        <v>1.001600242382305e-10</v>
+        <v>1.001600242382333e-10</v>
       </c>
       <c r="O9">
-        <v>4.356118579638462e-05</v>
+        <v>4.356118579638399e-05</v>
       </c>
       <c r="P9">
         <v>9.807753391976785e-20</v>
@@ -1527,16 +1487,16 @@
         <v>5.479856550316257e-08</v>
       </c>
       <c r="B10">
-        <v>2.895919008037264e-06</v>
+        <v>2.895919008037269e-06</v>
       </c>
       <c r="C10">
-        <v>1.248606345056467e-05</v>
+        <v>1.248606345056469e-05</v>
       </c>
       <c r="D10">
-        <v>2.218524029222357e-07</v>
+        <v>2.218524029222345e-07</v>
       </c>
       <c r="E10">
-        <v>1.405365041953481e-21</v>
+        <v>1.405365041953491e-21</v>
       </c>
       <c r="F10">
         <v>0.04792428049144502</v>
@@ -1548,28 +1508,28 @@
         <v>4.447274957576378e-08</v>
       </c>
       <c r="I10">
-        <v>1.890687436451046e-05</v>
+        <v>1.890687436451033e-05</v>
       </c>
       <c r="J10">
         <v>2.55373212442336e-05</v>
       </c>
       <c r="K10">
-        <v>3.939026732318233e-08</v>
+        <v>3.939026732318205e-08</v>
       </c>
       <c r="L10">
         <v>2.211636350226715e-09</v>
       </c>
       <c r="M10">
-        <v>4.542500117007921e-08</v>
+        <v>4.542500117007906e-08</v>
       </c>
       <c r="N10">
-        <v>8.638245399959584e-11</v>
+        <v>8.638245399959615e-11</v>
       </c>
       <c r="O10">
         <v>4.45569250834907e-05</v>
       </c>
       <c r="P10">
-        <v>9.85946349580465e-20</v>
+        <v>9.85946349580479e-20</v>
       </c>
       <c r="Q10" t="s">
         <v>11</v>
@@ -1580,19 +1540,19 @@
         <v>5.472288754799019e-08</v>
       </c>
       <c r="B11">
-        <v>2.722439150827053e-06</v>
+        <v>2.722439150827058e-06</v>
       </c>
       <c r="C11">
-        <v>4.295780970943577e-05</v>
+        <v>4.29578097093822e-05</v>
       </c>
       <c r="D11">
-        <v>1.233370982234454e-08</v>
+        <v>1.233370982238411e-08</v>
       </c>
       <c r="E11">
-        <v>1.734601305261118e-05</v>
+        <v>1.734601305255485e-05</v>
       </c>
       <c r="F11">
-        <v>0.04499115964694601</v>
+        <v>0.04499115964694617</v>
       </c>
       <c r="G11">
         <v>0.01050258470471664</v>
@@ -1601,28 +1561,28 @@
         <v>4.16356355615795e-08</v>
       </c>
       <c r="I11">
-        <v>9.867813066528182e-07</v>
+        <v>9.867813066559874e-07</v>
       </c>
       <c r="J11">
-        <v>1.251261554704541e-06</v>
+        <v>1.25126155470856e-06</v>
       </c>
       <c r="K11">
-        <v>2.053004585266921e-09</v>
+        <v>2.053004585273515e-09</v>
       </c>
       <c r="L11">
-        <v>1.080652623676399e-10</v>
+        <v>1.08065262367987e-10</v>
       </c>
       <c r="M11">
-        <v>2.5288596144602e-09</v>
+        <v>2.528859614468313e-09</v>
       </c>
       <c r="N11">
-        <v>2.971954319982985e-10</v>
+        <v>2.971954319979268e-10</v>
       </c>
       <c r="O11">
-        <v>2.932094654821369e-05</v>
+        <v>2.932094654823452e-05</v>
       </c>
       <c r="P11">
-        <v>6.765398695385759e-05</v>
+        <v>6.765398695385519e-05</v>
       </c>
       <c r="Q11" t="s">
         <v>11</v>
@@ -1630,52 +1590,52 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <v>5.471940890247937e-08</v>
+        <v>5.471940890247956e-08</v>
       </c>
       <c r="B12">
-        <v>2.722785342797729e-06</v>
+        <v>2.722785342797715e-06</v>
       </c>
       <c r="C12">
-        <v>7.104717707840947e-05</v>
+        <v>7.104717707827014e-05</v>
       </c>
       <c r="D12">
-        <v>2.226178028206273e-09</v>
+        <v>2.22617802822111e-09</v>
       </c>
       <c r="E12">
-        <v>4.988323497784697e-05</v>
+        <v>4.988323497739195e-05</v>
       </c>
       <c r="F12">
-        <v>0.04499402045303071</v>
+        <v>0.04499402045303055</v>
       </c>
       <c r="G12">
         <v>0.01050258484686324</v>
       </c>
       <c r="H12">
-        <v>4.163298941500336e-08</v>
+        <v>4.163298941500366e-08</v>
       </c>
       <c r="I12">
-        <v>1.781208231482807e-07</v>
+        <v>1.781208231494679e-07</v>
       </c>
       <c r="J12">
-        <v>2.258756913643002e-07</v>
+        <v>2.258756913658024e-07</v>
       </c>
       <c r="K12">
-        <v>3.705579121948515e-10</v>
+        <v>3.705579121973265e-10</v>
       </c>
       <c r="L12">
-        <v>1.950528451475127e-11</v>
+        <v>1.950528451488155e-11</v>
       </c>
       <c r="M12">
-        <v>4.564765739082778e-10</v>
+        <v>4.564765739113185e-10</v>
       </c>
       <c r="N12">
-        <v>4.915263749920553e-10</v>
+        <v>4.915263749910913e-10</v>
       </c>
       <c r="O12">
-        <v>1.447616570023402e-05</v>
+        <v>1.447616570027372e-05</v>
       </c>
       <c r="P12">
-        <v>3.51167650716732e-05</v>
+        <v>3.511676507158699e-05</v>
       </c>
       <c r="Q12" t="s">
         <v>11</v>
@@ -1696,239 +1656,239 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
+      <c r="A2">
+        <v>6.938893903907228e-17</v>
       </c>
       <c r="B2">
-        <v>4.083045303377627</v>
+        <v>6.938893903907228e-17</v>
       </c>
       <c r="C2">
-        <v>81.29446712796258</v>
+        <v>5.960929991798147e-15</v>
       </c>
       <c r="D2">
-        <v>0.0005624203012347578</v>
+        <v>3.112434423147188e-15</v>
       </c>
       <c r="E2">
-        <v>18.70497045762571</v>
+        <v>9.006852126169957e-30</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
+      <c r="A3">
+        <v>-1.249000902703301e-16</v>
       </c>
       <c r="B3">
-        <v>4.188505171866399</v>
+        <v>-1.249000902703301e-16</v>
       </c>
       <c r="C3">
-        <v>63.76775392067646</v>
+        <v>2.873271282358147e-16</v>
       </c>
       <c r="D3">
-        <v>0.0004411650710826132</v>
+        <v>1.549155497892335e-16</v>
       </c>
       <c r="E3">
-        <v>36.23180491453552</v>
+        <v>5.148973706319275e-31</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
+      <c r="A4">
+        <v>2.775557561562891e-17</v>
       </c>
       <c r="B4">
-        <v>4.317791703646318</v>
+        <v>4.163336342344337e-17</v>
       </c>
       <c r="C4">
-        <v>47.34941180805709</v>
+        <v>1.219727444046192e-18</v>
       </c>
       <c r="D4">
-        <v>0.0003275778954360868</v>
+        <v>6.911788849595091e-19</v>
       </c>
       <c r="E4">
-        <v>52.65026061404868</v>
+        <v>1.131483842327501e-33</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
+      <c r="A5">
+        <v>2.92377233535035e-13</v>
       </c>
       <c r="B5">
-        <v>4.453396906014182</v>
+        <v>2.922662112325725e-13</v>
       </c>
       <c r="C5">
-        <v>34.65049044643197</v>
+        <v>6.082039169172382e-13</v>
       </c>
       <c r="D5">
-        <v>0.0002397228244837235</v>
+        <v>4.587870881811451e-13</v>
       </c>
       <c r="E5">
-        <v>65.34927043314774</v>
+        <v>5.668986226512874e-28</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
+      <c r="A6">
+        <v>1.020017403874363e-14</v>
       </c>
       <c r="B6">
-        <v>4.577814929171851</v>
+        <v>1.015854067532018e-14</v>
       </c>
       <c r="C6">
-        <v>26.01904563842913</v>
+        <v>5.353980063113606e-15</v>
       </c>
       <c r="D6">
-        <v>0.0001800078160641847</v>
+        <v>8.086440588320198e-15</v>
       </c>
       <c r="E6">
-        <v>73.98077435914649</v>
+        <v>4.087690010464689e-30</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
+      <c r="A7">
+        <v>-2.775557561562891e-17</v>
       </c>
       <c r="B7">
-        <v>4.681178881169333</v>
+        <v>-2.775557561562891e-17</v>
       </c>
       <c r="C7">
-        <v>20.50819370856187</v>
+        <v>4.174178364069192e-18</v>
       </c>
       <c r="D7">
-        <v>0.0001418820356518795</v>
+        <v>1.127570259384925e-17</v>
       </c>
       <c r="E7">
-        <v>79.49166440940589</v>
+        <v>1.950004068692076e-33</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
+      <c r="A8">
+        <v>4.161254674173165e-13</v>
       </c>
       <c r="B8">
-        <v>4.766556609447368</v>
+        <v>4.16236489719779e-13</v>
       </c>
       <c r="C8">
-        <v>16.84805154806151</v>
+        <v>4.83901520199545e-14</v>
       </c>
       <c r="D8">
-        <v>0.0001165600386058768</v>
+        <v>2.705799451684088e-13</v>
       </c>
       <c r="E8">
-        <v>83.15183193939177</v>
+        <v>2.660622866216141e-29</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
+      <c r="A9">
+        <v>9.992007221626409e-16</v>
       </c>
       <c r="B9">
-        <v>4.839305579036515</v>
+        <v>1.02695629777827e-15</v>
       </c>
       <c r="C9">
-        <v>14.24953567645814</v>
+        <v>7.410521848938423e-17</v>
       </c>
       <c r="D9">
-        <v>9.858270102188038e-05</v>
+        <v>6.558745517179498e-16</v>
       </c>
       <c r="E9">
-        <v>85.75036574091459</v>
+        <v>3.473896137188477e-32</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
+      <c r="A10">
+        <v>1.804112415015879e-16</v>
       </c>
       <c r="B10">
-        <v>4.903574462440121</v>
+        <v>1.734723475976807e-16</v>
       </c>
       <c r="C10">
-        <v>12.28943253008334</v>
+        <v>9.486769009248164e-20</v>
       </c>
       <c r="D10">
-        <v>8.502210039330299e-05</v>
+        <v>4.472333961502706e-19</v>
       </c>
       <c r="E10">
-        <v>87.71048244781633</v>
+        <v>1.384262147528326e-33</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
+      <c r="A11">
+        <v>3.608224830031759e-16</v>
       </c>
       <c r="B11">
-        <v>4.366957870124041</v>
+        <v>3.885780586188048e-16</v>
       </c>
       <c r="C11">
-        <v>42.28130876912969</v>
+        <v>1.283234586299531e-15</v>
       </c>
       <c r="D11">
-        <v>0.0002925151889747032</v>
+        <v>2.738762450334165e-15</v>
       </c>
       <c r="E11">
-        <v>57.71839871695607</v>
+        <v>6.410033636695955e-15</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
+      <c r="A12">
+        <v>4.163336342344337e-16</v>
       </c>
       <c r="B12">
-        <v>4.148453173241441</v>
+        <v>3.469446951953614e-16</v>
       </c>
       <c r="C12">
-        <v>71.04717707840948</v>
+        <v>5.192583017211982e-15</v>
       </c>
       <c r="D12">
-        <v>0.0004915263749920553</v>
+        <v>4.174828885372683e-15</v>
       </c>
       <c r="E12">
-        <v>28.95233140046804</v>
+        <v>4.897894156224991e-14</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -1940,259 +1900,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>6.938893903907228e-17</v>
-      </c>
-      <c r="B2">
-        <v>6.938893903907228e-17</v>
-      </c>
-      <c r="C2">
-        <v>5.983752447528967e-15</v>
-      </c>
-      <c r="D2">
-        <v>3.124348788583267e-15</v>
-      </c>
-      <c r="E2">
-        <v>9.04153090223108e-30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>-1.249000902703301e-16</v>
-      </c>
-      <c r="B3">
-        <v>-1.249000902703301e-16</v>
-      </c>
-      <c r="C3">
-        <v>2.875846262517801e-16</v>
-      </c>
-      <c r="D3">
-        <v>1.550680157197393e-16</v>
-      </c>
-      <c r="E3">
-        <v>5.156436684853776e-31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>2.775557561562891e-17</v>
-      </c>
-      <c r="B4">
-        <v>4.163336342344337e-17</v>
-      </c>
-      <c r="C4">
-        <v>1.219727444046192e-18</v>
-      </c>
-      <c r="D4">
-        <v>6.844026213814747e-19</v>
-      </c>
-      <c r="E4">
-        <v>1.131483842327501e-33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>2.935152121352758e-13</v>
-      </c>
-      <c r="B5">
-        <v>2.936123566499305e-13</v>
-      </c>
-      <c r="C5">
-        <v>6.120426702341947e-13</v>
-      </c>
-      <c r="D5">
-        <v>4.617034429473324e-13</v>
-      </c>
-      <c r="E5">
-        <v>5.705119801905738e-28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>1.057487430955462e-14</v>
-      </c>
-      <c r="B6">
-        <v>1.051936315832336e-14</v>
-      </c>
-      <c r="C6">
-        <v>5.477958581537323e-15</v>
-      </c>
-      <c r="D6">
-        <v>8.274719071835884e-15</v>
-      </c>
-      <c r="E6">
-        <v>4.182758727344504e-30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>3.747002708109903e-16</v>
-      </c>
-      <c r="B7">
-        <v>3.747002708109903e-16</v>
-      </c>
-      <c r="C7">
-        <v>3.455894424797545e-18</v>
-      </c>
-      <c r="D7">
-        <v>1.147899050119028e-17</v>
-      </c>
-      <c r="E7">
-        <v>1.889818757929975e-33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>4.149180998780366e-13</v>
-      </c>
-      <c r="B8">
-        <v>4.149597332414601e-13</v>
-      </c>
-      <c r="C8">
-        <v>4.825175361263673e-14</v>
-      </c>
-      <c r="D8">
-        <v>2.698016912964715e-13</v>
-      </c>
-      <c r="E8">
-        <v>2.653013035523381e-29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>1.1518563880486e-15</v>
-      </c>
-      <c r="B9">
-        <v>1.110223024625157e-15</v>
-      </c>
-      <c r="C9">
-        <v>7.494547517306049e-17</v>
-      </c>
-      <c r="D9">
-        <v>6.589374228552214e-16</v>
-      </c>
-      <c r="E9">
-        <v>3.461859075036056e-32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>1.804112415015879e-16</v>
-      </c>
-      <c r="B10">
-        <v>1.734723475976807e-16</v>
-      </c>
-      <c r="C10">
-        <v>8.131516293641283e-20</v>
-      </c>
-      <c r="D10">
-        <v>5.827586677109586e-19</v>
-      </c>
-      <c r="E10">
-        <v>-1.203706215242022e-35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>1.942890293094024e-16</v>
-      </c>
-      <c r="B11">
-        <v>2.220446049250313e-16</v>
-      </c>
-      <c r="C11">
-        <v>1.295133705142559e-15</v>
-      </c>
-      <c r="D11">
-        <v>2.713066858846258e-15</v>
-      </c>
-      <c r="E11">
-        <v>6.468756736863202e-15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>5.828670879282072e-16</v>
-      </c>
-      <c r="B12">
-        <v>4.996003610813204e-16</v>
-      </c>
-      <c r="C12">
-        <v>5.252498739768963e-15</v>
-      </c>
-      <c r="D12">
-        <v>4.21862387687752e-15</v>
-      </c>
-      <c r="E12">
-        <v>4.952016173422752e-14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>